<commit_message>
Update G L PURAM - TEACHERS TABS DATA.xlsx
</commit_message>
<xml_diff>
--- a/BYJUS/G L PURAM - TEACHERS TABS DATA.xlsx
+++ b/BYJUS/G L PURAM - TEACHERS TABS DATA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MEO G L PURAM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\docs\BYJUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F422CB-A771-4C5D-B3C3-5EC369A567D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E96ECB-94F5-4951-9D74-DA9F4835B04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{E5CD553F-4CE9-4630-A9F3-87EFCB4DAB9B}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MANYAM (2)'!$B$2:$K$50</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="101">
   <si>
     <t>district_name</t>
   </si>
@@ -305,6 +307,39 @@
   </si>
   <si>
     <t>R9ZTB07Y3VR</t>
+  </si>
+  <si>
+    <t>R9ZTB07YTKA</t>
+  </si>
+  <si>
+    <t>R9ZTB07YOEA</t>
+  </si>
+  <si>
+    <t>R9ZTB093ADE</t>
+  </si>
+  <si>
+    <t>R9ZTB092JAZ</t>
+  </si>
+  <si>
+    <t>R9ZTB08XSYD</t>
+  </si>
+  <si>
+    <t>R9ZTB07X138</t>
+  </si>
+  <si>
+    <t>R9ZTB0EX17T</t>
+  </si>
+  <si>
+    <t>R9ZTB07WZZZ</t>
+  </si>
+  <si>
+    <t>R9ZTB0EZPWP</t>
+  </si>
+  <si>
+    <t>R9ZTB0EWB5A</t>
+  </si>
+  <si>
+    <t>R9ZTB0EZDWE</t>
   </si>
 </sst>
 </file>
@@ -342,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -365,11 +400,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -389,6 +463,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,15 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216B0B0F-64BF-4DAE-B8B1-F0D76D10B71C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane xSplit="3" ySplit="35" topLeftCell="K36" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="G1" sqref="G1"/>
-      <selection pane="topRight" activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
-      <selection pane="bottomRight" activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +922,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -885,7 +964,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -923,7 +1002,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -961,7 +1040,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -999,7 +1078,7 @@
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1037,7 +1116,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1075,7 +1154,7 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1113,7 +1192,7 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1151,7 +1230,7 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1189,7 +1268,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1227,7 +1306,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1261,11 +1340,15 @@
       <c r="K13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="L13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1237294987</v>
+      </c>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1299,11 +1382,15 @@
       <c r="K14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1156708174</v>
+      </c>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1341,7 +1428,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1379,7 +1466,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1417,7 +1504,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1455,7 +1542,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1493,7 +1580,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1531,7 +1618,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1569,7 +1656,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1607,7 +1694,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1645,7 +1732,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1683,7 +1770,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1721,7 +1808,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -1759,7 +1846,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -1797,7 +1884,7 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
-    <row r="28" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1835,7 +1922,7 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
-    <row r="29" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -1873,7 +1960,7 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -1911,7 +1998,7 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
-    <row r="31" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -1949,7 +2036,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -1987,7 +2074,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -2025,7 +2112,7 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2063,7 +2150,7 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2178,7 +2265,9 @@
       <c r="L37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="M37" s="3"/>
+      <c r="M37" s="3">
+        <v>1319867385</v>
+      </c>
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2218,7 +2307,9 @@
       <c r="L38" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="M38" s="3"/>
+      <c r="M38" s="3">
+        <v>1150325400</v>
+      </c>
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2258,10 +2349,12 @@
       <c r="L39" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="M39" s="3"/>
+      <c r="M39" s="3">
+        <v>2013408235</v>
+      </c>
       <c r="N39" s="3"/>
     </row>
-    <row r="40" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -2299,7 +2392,7 @@
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
     </row>
-    <row r="41" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -2337,7 +2430,7 @@
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
     </row>
-    <row r="42" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -2371,11 +2464,15 @@
       <c r="K42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
+      <c r="L42" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M42" s="3">
+        <v>1830560308</v>
+      </c>
       <c r="N42" s="3"/>
     </row>
-    <row r="43" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -2409,11 +2506,15 @@
       <c r="K43" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
+      <c r="L43" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="M43" s="3">
+        <v>1840809074</v>
+      </c>
       <c r="N43" s="3"/>
     </row>
-    <row r="44" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -2447,11 +2548,15 @@
       <c r="K44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
+      <c r="L44" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="M44" s="10">
+        <v>1914549191</v>
+      </c>
       <c r="N44" s="3"/>
     </row>
-    <row r="45" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -2482,14 +2587,18 @@
       <c r="J45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-    </row>
-    <row r="46" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K45" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L45" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="M45" s="11">
+        <v>1792308990</v>
+      </c>
+      <c r="N45" s="9"/>
+    </row>
+    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -2520,14 +2629,18 @@
       <c r="J46" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K46" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-    </row>
-    <row r="47" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L46" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="M46" s="11">
+        <v>1589589715</v>
+      </c>
+      <c r="N46" s="9"/>
+    </row>
+    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -2558,14 +2671,18 @@
       <c r="J47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K47" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-    </row>
-    <row r="48" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K47" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L47" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="M47" s="11">
+        <v>1203415760</v>
+      </c>
+      <c r="N47" s="9"/>
+    </row>
+    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -2596,14 +2713,18 @@
       <c r="J48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-    </row>
-    <row r="49" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K48" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M48" s="11">
+        <v>1682524602</v>
+      </c>
+      <c r="N48" s="9"/>
+    </row>
+    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -2634,14 +2755,18 @@
       <c r="J49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-    </row>
-    <row r="50" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K49" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L49" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="M49" s="11">
+        <v>1398960908</v>
+      </c>
+      <c r="N49" s="9"/>
+    </row>
+    <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -2672,21 +2797,19 @@
       <c r="J50" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K50" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
+      <c r="K50" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L50" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="M50" s="11">
+        <v>1227631226</v>
+      </c>
+      <c r="N50" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:K50" xr:uid="{216B0B0F-64BF-4DAE-B8B1-F0D76D10B71C}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="GTWAHSGIRLS  REGIDI"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B2:K50" xr:uid="{216B0B0F-64BF-4DAE-B8B1-F0D76D10B71C}"/>
   <conditionalFormatting sqref="H2">
     <cfRule type="duplicateValues" dxfId="5" priority="4"/>
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
@@ -2698,6 +2821,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>